<commit_message>
update the analysis with only 20 selected quant-seq samples
</commit_message>
<xml_diff>
--- a/exp_design/NGS_samplesheet_mRNAseq_2020.xlsx
+++ b/exp_design/NGS_samplesheet_mRNAseq_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Philipp/smallRNA_analysis_philipp/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E298E6D4-8699-4349-8076-34F94ED21CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BF7485-DBAF-9340-9728-2BB34D6190B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32140" yWindow="-11020" windowWidth="39860" windowHeight="24640" activeTab="1" xr2:uid="{E0B57B85-6670-D140-A58F-1C91E8E5F633}"/>
+    <workbookView xWindow="32160" yWindow="-10620" windowWidth="41600" windowHeight="24640" activeTab="1" xr2:uid="{E0B57B85-6670-D140-A58F-1C91E8E5F633}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3154,7 +3154,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>

</xml_diff>